<commit_message>
Updated story points and format
</commit_message>
<xml_diff>
--- a/Rent-a-Car Sprint #1 Backlog.xlsx
+++ b/Rent-a-Car Sprint #1 Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Antonio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\Summer 2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>Rent-a-Car - Sprint 1</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Feature Burndown - Based on estimated hours remaining</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
@@ -185,16 +182,85 @@
     <t>Allow input for the customer's email address</t>
   </si>
   <si>
-    <t>Get a customer's first and last name, age, phone number, and email</t>
-  </si>
-  <si>
-    <t>As a customer storage system, I want to receive a customer's information so that car may be rented.</t>
-  </si>
-  <si>
     <t>Requirement</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>(name)</t>
+  </si>
+  <si>
+    <t>When I enter the customer's information, the car should be rented.</t>
+  </si>
+  <si>
+    <t>When I add a car to the inventory, all its information is recorded.</t>
+  </si>
+  <si>
+    <t>When the customer's information is received, the car will be rented.</t>
+  </si>
+  <si>
+    <t>[Burndown chart goes here and shows hours and story points]</t>
+  </si>
+  <si>
+    <t>(planned hours</t>
+  </si>
+  <si>
+    <t>for each day</t>
+  </si>
+  <si>
+    <t>and task)</t>
+  </si>
+  <si>
+    <t>Input the customer's first name</t>
+  </si>
+  <si>
+    <t>Input the customer's last name</t>
+  </si>
+  <si>
+    <t>Input the customer's phone number</t>
+  </si>
+  <si>
+    <t>Input the customer's email address</t>
+  </si>
+  <si>
+    <t>Input or choose the customer's age</t>
+  </si>
+  <si>
+    <t>Give the car's brand a value and store it</t>
+  </si>
+  <si>
+    <t>Give the car's model a value and store it</t>
+  </si>
+  <si>
+    <t>Give the car's color a value and store it</t>
+  </si>
+  <si>
+    <t>Give the car's year a value and store it</t>
+  </si>
+  <si>
+    <t>Give the car's availability a value and store it</t>
+  </si>
+  <si>
+    <t>Give the car's daily price a value and store it</t>
+  </si>
+  <si>
+    <t>Store the customer's first name</t>
+  </si>
+  <si>
+    <t>Store the customer's last name</t>
+  </si>
+  <si>
+    <t>Store the customer's age</t>
+  </si>
+  <si>
+    <t>Store the customer's phone number</t>
+  </si>
+  <si>
+    <t>Store the customer's email address</t>
+  </si>
+  <si>
+    <t>Get customer's first name and last name, age, phone number, and email</t>
   </si>
   <si>
     <t>Record the customer's first name</t>
@@ -212,91 +278,10 @@
     <t>Record the customer's email address</t>
   </si>
   <si>
-    <t>Issues</t>
-  </si>
-  <si>
-    <t>(name)</t>
-  </si>
-  <si>
-    <t>(issue)</t>
-  </si>
-  <si>
-    <t>(…)</t>
-  </si>
-  <si>
-    <t>When I enter the customer's information, the car should be rented.</t>
-  </si>
-  <si>
-    <t>When I add a car to the inventory, all its information is recorded.</t>
-  </si>
-  <si>
-    <t>When the customer's information is received, the car will be rented.</t>
-  </si>
-  <si>
-    <t>[Burndown chart goes here and shows hours and story points]</t>
-  </si>
-  <si>
-    <t>(planned hours</t>
-  </si>
-  <si>
-    <t>for each day</t>
-  </si>
-  <si>
-    <t>and task)</t>
-  </si>
-  <si>
-    <t>Input the customer's first name</t>
-  </si>
-  <si>
-    <t>Input the customer's last name</t>
-  </si>
-  <si>
-    <t>Input the customer's phone number</t>
-  </si>
-  <si>
-    <t>Input the customer's email address</t>
-  </si>
-  <si>
-    <t>Input or choose the customer's age</t>
-  </si>
-  <si>
-    <t>Give the car's brand a value and store it</t>
-  </si>
-  <si>
-    <t>Give the car's model a value and store it</t>
-  </si>
-  <si>
-    <t>Give the car's color a value and store it</t>
-  </si>
-  <si>
-    <t>Give the car's year a value and store it</t>
-  </si>
-  <si>
-    <t>Give the car's availability a value and store it</t>
-  </si>
-  <si>
-    <t>Give the car's daily price a value and store it</t>
-  </si>
-  <si>
-    <t>Store the customer's first name</t>
-  </si>
-  <si>
-    <t>Store the customer's last name</t>
-  </si>
-  <si>
-    <t>Store the customer's age</t>
-  </si>
-  <si>
-    <t>Store the customer's phone number</t>
-  </si>
-  <si>
-    <t>Store the customer's email address</t>
-  </si>
-  <si>
-    <t>(expected detail)</t>
-  </si>
-  <si>
-    <t>(any scale)</t>
+    <t>As a customer storage system, I want to receive a customer's information so that the car may be rented.</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -493,7 +478,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,6 +563,18 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -616,13 +613,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -699,13 +690,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -750,13 +735,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -801,13 +780,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Connector 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -852,13 +825,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Connector 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -903,13 +870,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Straight Connector 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -954,13 +915,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Straight Connector 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1005,13 +960,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Connector 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="20" name="Straight Connector 19"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1056,13 +1005,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Straight Connector 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1107,13 +1050,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="Straight Connector 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1158,13 +1095,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Straight Connector 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1209,13 +1140,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="Straight Connector 23">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1260,13 +1185,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Straight Connector 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1311,13 +1230,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Straight Connector 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1362,13 +1275,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="Straight Connector 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1413,13 +1320,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="Straight Connector 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1464,13 +1365,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Straight Connector 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="29" name="Straight Connector 28"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1515,13 +1410,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Straight Connector 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="30" name="Straight Connector 29"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1566,13 +1455,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Straight Connector 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1617,13 +1500,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="Straight Connector 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="32" name="Straight Connector 31"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1668,13 +1545,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Straight Connector 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1719,13 +1590,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Straight Connector 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1770,13 +1635,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="38" name="Straight Connector 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1821,13 +1680,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Straight Connector 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="39" name="Straight Connector 38"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1872,19 +1725,958 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="Straight Connector 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="40" name="Straight Connector 39"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="9136380"/>
           <a:ext cx="29862780" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6370320"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6560820"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6758940"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6957060"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7155180"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7353300"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Connector 44"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7551420"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Connector 45"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7947660"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Connector 46"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8145780"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Connector 47"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8343900"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Straight Connector 48"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8542020"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Connector 49"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8740140"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Connector 50"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8938260"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Straight Connector 51"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9334500"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Connector 52"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9532620"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Connector 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9730740"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Straight Connector 54"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9928860"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Connector 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10126980"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Straight Connector 56"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10325100"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Connector 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10721340"/>
+          <a:ext cx="30396180" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Connector 58"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10919460"/>
+          <a:ext cx="30396180" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2210,44 +3002,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" customWidth="1"/>
-    <col min="3" max="3" width="96.7109375" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" customWidth="1"/>
+    <col min="3" max="3" width="96.6640625" customWidth="1"/>
+    <col min="4" max="4" width="60.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" customWidth="1"/>
+    <col min="15" max="15" width="14.21875" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.77734375" customWidth="1"/>
+    <col min="19" max="19" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
@@ -2259,7 +3049,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -2283,13 +3073,13 @@
         <v>4</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>8</v>
@@ -2298,7 +3088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
@@ -2312,29 +3102,29 @@
         <v>11</v>
       </c>
       <c r="I5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="N5" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>38</v>
       </c>
       <c r="O5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2350,7 +3140,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2375,12 +3165,16 @@
       <c r="L7" s="1">
         <v>4</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="M7" s="1">
+        <v>14</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +3190,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2430,27 +3224,27 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="O10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="O11" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>20</v>
       </c>
@@ -2509,30 +3303,30 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="32">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="31" t="s">
-        <v>89</v>
+      <c r="F29" s="32">
+        <v>2</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -2543,27 +3337,29 @@
       <c r="O29" s="31"/>
       <c r="P29" s="31"/>
       <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
+      <c r="R29" s="31" t="s">
+        <v>85</v>
+      </c>
       <c r="S29" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="33"/>
       <c r="B30" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D30" s="33"/>
-      <c r="E30" s="33" t="s">
-        <v>55</v>
+      <c r="E30" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
       <c r="H30" s="35" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
@@ -2577,22 +3373,22 @@
       <c r="R30" s="33"/>
       <c r="S30" s="33"/>
     </row>
-    <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="33"/>
       <c r="B31" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D31" s="33"/>
-      <c r="E31" s="33" t="s">
-        <v>55</v>
+      <c r="E31" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
       <c r="H31" s="35" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
@@ -2606,17 +3402,17 @@
       <c r="R31" s="33"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="33"/>
       <c r="B32" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D32" s="33"/>
-      <c r="E32" s="33" t="s">
-        <v>55</v>
+      <c r="E32" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="33"/>
@@ -2633,17 +3429,17 @@
       <c r="R32" s="33"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="33"/>
       <c r="B33" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D33" s="33"/>
-      <c r="E33" s="33" t="s">
-        <v>55</v>
+      <c r="E33" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
@@ -2660,17 +3456,17 @@
       <c r="R33" s="33"/>
       <c r="S33" s="33"/>
     </row>
-    <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="33"/>
       <c r="B34" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D34" s="33"/>
-      <c r="E34" s="33" t="s">
-        <v>55</v>
+      <c r="E34" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
@@ -2687,17 +3483,17 @@
       <c r="R34" s="33"/>
       <c r="S34" s="33"/>
     </row>
-    <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
       <c r="B35" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D35" s="33"/>
-      <c r="E35" s="33" t="s">
-        <v>55</v>
+      <c r="E35" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
@@ -2714,7 +3510,7 @@
       <c r="R35" s="33"/>
       <c r="S35" s="33"/>
     </row>
-    <row r="36" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -2735,27 +3531,27 @@
       <c r="R36" s="20"/>
       <c r="S36" s="20"/>
     </row>
-    <row r="37" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="32">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B37" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="31" t="s">
-        <v>47</v>
-      </c>
       <c r="D37" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F37" s="31" t="s">
-        <v>90</v>
+      <c r="F37" s="32">
+        <v>2</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H37" s="31"/>
       <c r="I37" s="31"/>
@@ -2767,22 +3563,24 @@
       <c r="O37" s="31"/>
       <c r="P37" s="31"/>
       <c r="Q37" s="31"/>
-      <c r="R37" s="31"/>
+      <c r="R37" s="31" t="s">
+        <v>85</v>
+      </c>
       <c r="S37" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="33"/>
       <c r="B38" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D38" s="33"/>
-      <c r="E38" s="33" t="s">
-        <v>55</v>
+      <c r="E38" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F38" s="33"/>
       <c r="G38" s="33"/>
@@ -2799,17 +3597,17 @@
       <c r="R38" s="33"/>
       <c r="S38" s="33"/>
     </row>
-    <row r="39" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="33"/>
       <c r="B39" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D39" s="33"/>
-      <c r="E39" s="33" t="s">
-        <v>55</v>
+      <c r="E39" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F39" s="33"/>
       <c r="G39" s="33"/>
@@ -2826,17 +3624,17 @@
       <c r="R39" s="33"/>
       <c r="S39" s="33"/>
     </row>
-    <row r="40" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="33"/>
       <c r="B40" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D40" s="33"/>
-      <c r="E40" s="33" t="s">
-        <v>55</v>
+      <c r="E40" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
@@ -2853,17 +3651,17 @@
       <c r="R40" s="33"/>
       <c r="S40" s="33"/>
     </row>
-    <row r="41" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="33"/>
       <c r="B41" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D41" s="33"/>
-      <c r="E41" s="33" t="s">
-        <v>55</v>
+      <c r="E41" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F41" s="33"/>
       <c r="G41" s="33"/>
@@ -2880,17 +3678,17 @@
       <c r="R41" s="33"/>
       <c r="S41" s="33"/>
     </row>
-    <row r="42" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="33"/>
       <c r="B42" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="33"/>
+      <c r="E42" s="36" t="s">
         <v>52</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33" t="s">
-        <v>55</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
@@ -2907,7 +3705,7 @@
       <c r="R42" s="33"/>
       <c r="S42" s="33"/>
     </row>
-    <row r="43" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -2928,25 +3726,27 @@
       <c r="R43" s="20"/>
       <c r="S43" s="20"/>
     </row>
-    <row r="44" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="32">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C44" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="32">
+        <v>2</v>
+      </c>
+      <c r="G44" s="31" t="s">
         <v>54</v>
-      </c>
-      <c r="D44" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31" t="s">
-        <v>63</v>
       </c>
       <c r="H44" s="31"/>
       <c r="I44" s="31"/>
@@ -2958,22 +3758,24 @@
       <c r="O44" s="31"/>
       <c r="P44" s="31"/>
       <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
+      <c r="R44" s="31" t="s">
+        <v>85</v>
+      </c>
       <c r="S44" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="33"/>
       <c r="B45" s="33" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D45" s="33"/>
-      <c r="E45" s="33" t="s">
-        <v>55</v>
+      <c r="E45" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
@@ -2990,17 +3792,17 @@
       <c r="R45" s="33"/>
       <c r="S45" s="33"/>
     </row>
-    <row r="46" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="33"/>
       <c r="B46" s="33" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D46" s="33"/>
-      <c r="E46" s="33" t="s">
-        <v>55</v>
+      <c r="E46" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F46" s="33"/>
       <c r="G46" s="33"/>
@@ -3017,17 +3819,17 @@
       <c r="R46" s="33"/>
       <c r="S46" s="33"/>
     </row>
-    <row r="47" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="33"/>
       <c r="B47" s="33" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D47" s="33"/>
-      <c r="E47" s="33" t="s">
-        <v>55</v>
+      <c r="E47" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F47" s="33"/>
       <c r="G47" s="33"/>
@@ -3044,17 +3846,17 @@
       <c r="R47" s="33"/>
       <c r="S47" s="33"/>
     </row>
-    <row r="48" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="33"/>
       <c r="B48" s="33" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D48" s="33"/>
-      <c r="E48" s="33" t="s">
-        <v>55</v>
+      <c r="E48" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
@@ -3071,17 +3873,17 @@
       <c r="R48" s="33"/>
       <c r="S48" s="33"/>
     </row>
-    <row r="49" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="33"/>
       <c r="B49" s="33" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D49" s="33"/>
-      <c r="E49" s="33" t="s">
-        <v>55</v>
+      <c r="E49" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="F49" s="33"/>
       <c r="G49" s="33"/>
@@ -3098,7 +3900,7 @@
       <c r="R49" s="33"/>
       <c r="S49" s="33"/>
     </row>
-    <row r="50" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
@@ -3119,7 +3921,7 @@
       <c r="R50" s="20"/>
       <c r="S50" s="20"/>
     </row>
-    <row r="51" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>30</v>
       </c>
@@ -3129,20 +3931,20 @@
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
       <c r="R51" s="21"/>
       <c r="S51" s="21"/>
     </row>
-    <row r="52" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>31</v>
       </c>
@@ -3152,20 +3954,20 @@
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="38"/>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38"/>
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
     </row>
-    <row r="53" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="26" t="s">
         <v>32</v>
       </c>
@@ -3175,20 +3977,40 @@
       <c r="E53" s="23"/>
       <c r="F53" s="23"/>
       <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="23"/>
-      <c r="M53" s="23"/>
-      <c r="N53" s="23"/>
-      <c r="O53" s="23"/>
-      <c r="P53" s="23"/>
-      <c r="Q53" s="23"/>
+      <c r="H53" s="39">
+        <v>6</v>
+      </c>
+      <c r="I53" s="39">
+        <v>6</v>
+      </c>
+      <c r="J53" s="39">
+        <v>6</v>
+      </c>
+      <c r="K53" s="39">
+        <v>6</v>
+      </c>
+      <c r="L53" s="39">
+        <v>6</v>
+      </c>
+      <c r="M53" s="39">
+        <v>6</v>
+      </c>
+      <c r="N53" s="39">
+        <v>4</v>
+      </c>
+      <c r="O53" s="39">
+        <v>2</v>
+      </c>
+      <c r="P53" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="39">
+        <v>0</v>
+      </c>
       <c r="R53" s="23"/>
       <c r="S53" s="23"/>
     </row>
-    <row r="54" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G54" s="11" t="s">
         <v>33</v>
       </c>
@@ -3223,7 +4045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
@@ -3244,9 +4066,9 @@
       <c r="R55" s="20"/>
       <c r="S55" s="20"/>
     </row>
-    <row r="56" spans="1:19" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="28" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -3266,7 +4088,7 @@
       <c r="R56" s="20"/>
       <c r="S56" s="20"/>
     </row>
-    <row r="57" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="30" t="s">
         <v>14</v>
       </c>
@@ -3288,10 +4110,8 @@
       <c r="R57" s="20"/>
       <c r="S57" s="20"/>
     </row>
-    <row r="58" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="58" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="29"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
@@ -3311,10 +4131,8 @@
       <c r="R58" s="20"/>
       <c r="S58" s="20"/>
     </row>
-    <row r="59" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="59" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="29"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
       <c r="D59" s="20"/>
@@ -3334,10 +4152,8 @@
       <c r="R59" s="20"/>
       <c r="S59" s="20"/>
     </row>
-    <row r="60" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
-        <v>65</v>
-      </c>
+    <row r="60" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="29"/>
       <c r="B60" s="20"/>
       <c r="C60" s="20"/>
       <c r="D60" s="20"/>
@@ -3357,7 +4173,7 @@
       <c r="R60" s="20"/>
       <c r="S60" s="20"/>
     </row>
-    <row r="61" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="29"/>
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
@@ -3378,7 +4194,7 @@
       <c r="R61" s="20"/>
       <c r="S61" s="20"/>
     </row>
-    <row r="62" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="29"/>
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
@@ -3399,7 +4215,7 @@
       <c r="R62" s="20"/>
       <c r="S62" s="20"/>
     </row>
-    <row r="63" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A63" s="30" t="s">
         <v>15</v>
       </c>
@@ -3422,33 +4238,27 @@
       <c r="R63" s="20"/>
       <c r="S63" s="20"/>
     </row>
-    <row r="64" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="64" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="29"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
     </row>
-    <row r="65" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="29"/>
+    </row>
+    <row r="66" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="29"/>
+    </row>
+    <row r="67" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="29"/>
     </row>
-    <row r="68" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="29"/>
     </row>
-    <row r="69" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="30" t="s">
         <v>16</v>
       </c>
@@ -3471,10 +4281,8 @@
       <c r="R69" s="20"/>
       <c r="S69" s="20"/>
     </row>
-    <row r="70" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="70" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="29"/>
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
       <c r="D70" s="20"/>
@@ -3494,10 +4302,8 @@
       <c r="R70" s="20"/>
       <c r="S70" s="20"/>
     </row>
-    <row r="71" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="71" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="29"/>
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
       <c r="D71" s="20"/>
@@ -3517,10 +4323,8 @@
       <c r="R71" s="20"/>
       <c r="S71" s="20"/>
     </row>
-    <row r="72" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
-        <v>65</v>
-      </c>
+    <row r="72" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="29"/>
       <c r="B72" s="20"/>
       <c r="C72" s="20"/>
       <c r="D72" s="20"/>
@@ -3540,7 +4344,7 @@
       <c r="R72" s="20"/>
       <c r="S72" s="20"/>
     </row>
-    <row r="73" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="29"/>
       <c r="B73" s="20"/>
       <c r="C73" s="20"/>
@@ -3561,7 +4365,7 @@
       <c r="R73" s="20"/>
       <c r="S73" s="20"/>
     </row>
-    <row r="74" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="29"/>
       <c r="B74" s="20"/>
       <c r="C74" s="20"/>
@@ -3582,7 +4386,7 @@
       <c r="R74" s="20"/>
       <c r="S74" s="20"/>
     </row>
-    <row r="75" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="30" t="s">
         <v>17</v>
       </c>
@@ -3605,10 +4409,8 @@
       <c r="R75" s="20"/>
       <c r="S75" s="20"/>
     </row>
-    <row r="76" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="76" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="29"/>
       <c r="B76" s="20"/>
       <c r="C76" s="20"/>
       <c r="D76" s="20"/>
@@ -3628,10 +4430,8 @@
       <c r="R76" s="20"/>
       <c r="S76" s="20"/>
     </row>
-    <row r="77" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="29" t="s">
-        <v>64</v>
-      </c>
+    <row r="77" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="29"/>
       <c r="B77" s="20"/>
       <c r="C77" s="20"/>
       <c r="D77" s="20"/>
@@ -3651,10 +4451,8 @@
       <c r="R77" s="20"/>
       <c r="S77" s="20"/>
     </row>
-    <row r="78" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="s">
-        <v>65</v>
-      </c>
+    <row r="78" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="29"/>
       <c r="B78" s="20"/>
       <c r="C78" s="20"/>
       <c r="D78" s="20"/>
@@ -3674,7 +4472,7 @@
       <c r="R78" s="20"/>
       <c r="S78" s="20"/>
     </row>
-    <row r="79" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="29"/>
       <c r="B79" s="20"/>
       <c r="C79" s="20"/>
@@ -3695,7 +4493,7 @@
       <c r="R79" s="20"/>
       <c r="S79" s="20"/>
     </row>
-    <row r="80" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="29"/>
       <c r="B80" s="20"/>
       <c r="C80" s="20"/>
@@ -3716,7 +4514,7 @@
       <c r="R80" s="20"/>
       <c r="S80" s="20"/>
     </row>
-    <row r="81" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="29"/>
       <c r="B81" s="20"/>
       <c r="C81" s="20"/>
@@ -3737,61 +4535,61 @@
       <c r="R81" s="20"/>
       <c r="S81" s="20"/>
     </row>
-    <row r="82" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="29"/>
     </row>
-    <row r="83" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="29"/>
     </row>
-    <row r="84" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="29"/>
     </row>
-    <row r="85" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="29"/>
     </row>
-    <row r="86" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="29"/>
     </row>
-    <row r="87" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="29"/>
     </row>
-    <row r="88" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="29"/>
     </row>
-    <row r="89" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="29"/>
     </row>
-    <row r="90" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="29"/>
     </row>
-    <row r="91" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="29"/>
     </row>
-    <row r="92" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="29"/>
     </row>
-    <row r="93" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="29"/>
     </row>
-    <row r="94" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="29"/>
     </row>
-    <row r="95" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="29"/>
     </row>
-    <row r="96" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="29"/>
     </row>
-    <row r="97" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="29"/>
     </row>
-    <row r="98" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="29"/>
     </row>
-    <row r="99" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="29"/>
     </row>
-    <row r="100" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="29"/>
     </row>
   </sheetData>

</xml_diff>